<commit_message>
Add data sizes and load times and data scan sizes for avro, parquet, json, csv, hudi, delta lake, iceberg and their related compression types.
</commit_message>
<xml_diff>
--- a/aws_glue_s3_destination_file_properties.xlsx
+++ b/aws_glue_s3_destination_file_properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earln\Documents\AWS\cloudnotes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6E1FED-58DB-4A7D-998F-16B9A9B6E353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E0CCC4-B104-4880-B198-85374E3C7C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22500" yWindow="-26328" windowWidth="46296" windowHeight="25536" xr2:uid="{7AAB3D60-D17A-4906-8409-7A274DB37C5C}"/>
+    <workbookView xWindow="-19670" yWindow="-21710" windowWidth="38620" windowHeight="21220" xr2:uid="{7AAB3D60-D17A-4906-8409-7A274DB37C5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="119">
   <si>
     <t>CSV</t>
   </si>
@@ -276,12 +276,274 @@
   <si>
     <t>For AWS Glue destinations that are in S3</t>
   </si>
+  <si>
+    <t>File Count</t>
+  </si>
+  <si>
+    <t>Record Count</t>
+  </si>
+  <si>
+    <t>Full Scan Time in Queue (ms)</t>
+  </si>
+  <si>
+    <t>Full Scan Run Time (sec)</t>
+  </si>
+  <si>
+    <t>Data scanned (MB)</t>
+  </si>
+  <si>
+    <t>Total Size (B)</t>
+  </si>
+  <si>
+    <t>Avg. File Size (B)</t>
+  </si>
+  <si>
+    <t>Job Run Time ([h]:mi:ss)</t>
+  </si>
+  <si>
+    <t>Worker Type: G.1X</t>
+  </si>
+  <si>
+    <t>Max capacity: 10 DPUs</t>
+  </si>
+  <si>
+    <t>Number of workers: 10</t>
+  </si>
+  <si>
+    <t>Job Name</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtocsvgzip</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtojsonuncompressednoindex</t>
+  </si>
+  <si>
+    <t>Original data populated by PricingTrxGenerator.py</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtocsvbzip2noindex</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtojsongzipnoindex</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtojsonbzip2noindex</t>
+  </si>
+  <si>
+    <t>Job Script Name</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtocsvbzip2noindex.py</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtocsvgzip.py</t>
+  </si>
+  <si>
+    <t>pricingtrxwheadercsvtojsonuncompressednorootindex.py</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtojsongzipnoindex.py</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtojsonbzip2noindex.py</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoavrononenoindex.py</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoavrobzip2noindex.py</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoavrogzipnoindex.py</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoorcnonenoindex.py</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoorcsnappynoindex.py</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoparquetsnappynoindex.py</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoorclzonoindex.py</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoorcgzipnoindex.py</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoorcuncompressednoindex.py</t>
+  </si>
+  <si>
+    <t>Table Name</t>
+  </si>
+  <si>
+    <t>pricingtrxwheadercsv</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvgzip</t>
+  </si>
+  <si>
+    <t>pricingtrxwheaderjsonuncompressed</t>
+  </si>
+  <si>
+    <t>pricingtrxjsongzipnonindex</t>
+  </si>
+  <si>
+    <t>pricingtrxjsonbzip2noindex</t>
+  </si>
+  <si>
+    <t>pricingtrxwheadercsvbzip2</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Need two Glue table properties to work correctly:  field.delim = , and skip.header.line.count = 1</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoavronone</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoavrobzip2</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoavrogzip</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoorcnone</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoorcsnappy</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoparquetsnappy</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoorclzo</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoorcgzip</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoorcuncompressed</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoparquetlzo</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoparquetgzip</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoparquetuncompressed</t>
+  </si>
+  <si>
+    <t>pricingtrxhudigzip</t>
+  </si>
+  <si>
+    <t>pricingtrxhudilzo</t>
+  </si>
+  <si>
+    <t>pricingtrxhudiuncompressed</t>
+  </si>
+  <si>
+    <t>pricingtrxhudisnappy</t>
+  </si>
+  <si>
+    <t>pricingtrxdeltalakesnappy</t>
+  </si>
+  <si>
+    <t>pricingtrxdeltalakeuncompressed</t>
+  </si>
+  <si>
+    <t>pricingtrxiceberggzip</t>
+  </si>
+  <si>
+    <t>pricingtrxiceberglzo</t>
+  </si>
+  <si>
+    <t>pricingtrxicebergsnappy</t>
+  </si>
+  <si>
+    <t>pricingtrxiceberguncompressed</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtohudigzip</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtohudilzo</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtohudisnappy</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtohudiuncompressed</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtodeltalakesnappy</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtodeltalakeuncompressed</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoiceberggzip</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoicebergsnappy</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoiceberglzo</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoiceberguncompressed</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtohudigzip.py</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtohudilzo.py</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtohudisnappy.py</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtohudiuncompressed.py</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtodeltalakesnappy.py</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtodeltalakeuncompressed.py</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoiceberggzip.py</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoiceberglzo.py</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoicebergsnappy.py</t>
+  </si>
+  <si>
+    <t>pricingtrxcsvtoiceberguncompressed.py</t>
+  </si>
+  <si>
+    <t>Hudi write op - insert; storage type = copy on write</t>
+  </si>
+  <si>
+    <t>How to query delta lake when there this no glue table?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,6 +566,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -313,7 +582,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -452,36 +721,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -794,119 +1090,281 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F349F45-06DF-4A85-93CA-17D22A2819FA}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="15.1328125" customWidth="1"/>
     <col min="2" max="2" width="19.3984375" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="12.796875" customWidth="1"/>
-    <col min="6" max="6" width="23.1328125" customWidth="1"/>
-    <col min="7" max="7" width="26.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="15" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="12.796875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="23.1328125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="26.53125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="13.19921875" customWidth="1"/>
+    <col min="10" max="11" width="11.86328125" customWidth="1"/>
+    <col min="12" max="12" width="33.1328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.1328125" style="20" customWidth="1"/>
+    <col min="14" max="14" width="15.1328125" customWidth="1"/>
+    <col min="15" max="15" width="12.06640625" customWidth="1"/>
+    <col min="16" max="16" width="11.53125" customWidth="1"/>
+    <col min="17" max="17" width="12.53125" customWidth="1"/>
+    <col min="18" max="18" width="41.796875" customWidth="1"/>
+    <col min="19" max="19" width="46.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.65">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.65">
+      <c r="A1" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="3" spans="1:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="11" t="s">
+    <row r="2" spans="1:19" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="H2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" s="9" t="s">
+      <c r="H3" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q3" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="S3" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" s="9"/>
-      <c r="B5" s="3" t="s">
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="16">
+        <v>12182</v>
+      </c>
+      <c r="I4" s="16">
+        <v>486906</v>
+      </c>
+      <c r="J4" s="17">
+        <v>46604041</v>
+      </c>
+      <c r="K4" s="17">
+        <v>3826</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="M4" s="21"/>
+      <c r="N4">
+        <v>95</v>
+      </c>
+      <c r="O4">
+        <v>14.218</v>
+      </c>
+      <c r="P4">
+        <v>44.45</v>
+      </c>
+      <c r="Q4" s="19">
+        <v>9.0393518518518522E-3</v>
+      </c>
+      <c r="R4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A5" s="13"/>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" s="10"/>
-      <c r="B6" s="5" t="s">
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="16">
+        <v>12182</v>
+      </c>
+      <c r="I5" s="16">
+        <v>486906</v>
+      </c>
+      <c r="J5" s="17">
+        <v>11850512</v>
+      </c>
+      <c r="K5">
+        <v>973</v>
+      </c>
+      <c r="L5" t="s">
+        <v>68</v>
+      </c>
+      <c r="M5" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="N5">
+        <v>99</v>
+      </c>
+      <c r="O5">
+        <v>15.488</v>
+      </c>
+      <c r="P5">
+        <v>11.3</v>
+      </c>
+      <c r="Q5" s="19">
+        <v>1.7222222222222222E-2</v>
+      </c>
+      <c r="R5" t="s">
+        <v>45</v>
+      </c>
+      <c r="S5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A6" s="12"/>
+      <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" s="8" t="s">
+      <c r="C6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="16">
+        <v>12182</v>
+      </c>
+      <c r="I6" s="16">
+        <v>486906</v>
+      </c>
+      <c r="J6" s="17">
+        <v>11999564</v>
+      </c>
+      <c r="K6">
+        <v>985</v>
+      </c>
+      <c r="L6" t="s">
+        <v>72</v>
+      </c>
+      <c r="M6" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="N6">
+        <v>118</v>
+      </c>
+      <c r="O6">
+        <v>15.792999999999999</v>
+      </c>
+      <c r="P6">
+        <v>11.44</v>
+      </c>
+      <c r="Q6" s="19">
+        <v>1.8067129629629631E-2</v>
+      </c>
+      <c r="R6" t="s">
+        <v>48</v>
+      </c>
+      <c r="S6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A8" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -927,60 +1385,151 @@
       <c r="G8" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" s="9"/>
-      <c r="B9" s="3" t="s">
+      <c r="H8" s="16">
+        <v>12182</v>
+      </c>
+      <c r="I8" s="16">
+        <v>486906</v>
+      </c>
+      <c r="J8" s="17">
+        <v>135828163</v>
+      </c>
+      <c r="K8" s="17">
+        <v>11150</v>
+      </c>
+      <c r="L8" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="M8" s="21"/>
+      <c r="N8">
+        <v>254</v>
+      </c>
+      <c r="O8">
+        <v>21.884</v>
+      </c>
+      <c r="P8">
+        <v>129.54</v>
+      </c>
+      <c r="Q8" s="18">
+        <v>1.8067129629629631E-2</v>
+      </c>
+      <c r="R8" t="s">
+        <v>46</v>
+      </c>
+      <c r="S8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A9" s="13"/>
+      <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A10" s="10"/>
-      <c r="B10" s="5" t="s">
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="22">
+        <v>12182</v>
+      </c>
+      <c r="I9" s="16">
+        <v>486906</v>
+      </c>
+      <c r="J9" s="17">
+        <v>14345687</v>
+      </c>
+      <c r="K9" s="17">
+        <v>1178</v>
+      </c>
+      <c r="L9" t="s">
+        <v>70</v>
+      </c>
+      <c r="N9">
+        <v>105</v>
+      </c>
+      <c r="O9">
+        <v>15.090999999999999</v>
+      </c>
+      <c r="P9">
+        <v>13.68</v>
+      </c>
+      <c r="Q9" s="19">
+        <v>1.7337962962962961E-2</v>
+      </c>
+      <c r="R9" t="s">
+        <v>49</v>
+      </c>
+      <c r="S9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A10" s="12"/>
+      <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A12" s="8" t="s">
+      <c r="C10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="22">
+        <v>12182</v>
+      </c>
+      <c r="I10" s="16">
+        <v>486906</v>
+      </c>
+      <c r="J10" s="17">
+        <v>13713152</v>
+      </c>
+      <c r="K10" s="17">
+        <v>1126</v>
+      </c>
+      <c r="L10" t="s">
+        <v>71</v>
+      </c>
+      <c r="N10">
+        <v>118</v>
+      </c>
+      <c r="O10">
+        <v>17.366</v>
+      </c>
+      <c r="P10">
+        <v>13.08</v>
+      </c>
+      <c r="Q10" s="19">
+        <v>1.7754629629629631E-2</v>
+      </c>
+      <c r="R10" t="s">
+        <v>50</v>
+      </c>
+      <c r="S10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A12" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1001,51 +1550,110 @@
       <c r="G12" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" s="9"/>
-      <c r="B13" s="3" t="s">
+      <c r="H12" s="17">
+        <v>12182</v>
+      </c>
+      <c r="I12" s="17">
+        <v>486906</v>
+      </c>
+      <c r="J12" s="17">
+        <v>62398096</v>
+      </c>
+      <c r="K12" s="17">
+        <v>5122</v>
+      </c>
+      <c r="L12" t="s">
+        <v>75</v>
+      </c>
+      <c r="N12">
+        <v>100</v>
+      </c>
+      <c r="O12">
+        <v>14.818</v>
+      </c>
+      <c r="P12">
+        <v>59.51</v>
+      </c>
+      <c r="Q12" s="19">
+        <v>1.7222222222222222E-2</v>
+      </c>
+      <c r="R12" t="s">
+        <v>75</v>
+      </c>
+      <c r="S12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A13" s="13"/>
+      <c r="B13" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A14" s="10"/>
-      <c r="B14" s="5" t="s">
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" t="s">
+        <v>76</v>
+      </c>
+      <c r="R13" t="s">
+        <v>76</v>
+      </c>
+      <c r="S13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A14" s="12"/>
+      <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A16" s="8" t="s">
+      <c r="C14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" t="s">
+        <v>77</v>
+      </c>
+      <c r="R14" t="s">
+        <v>77</v>
+      </c>
+      <c r="S14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A16" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1066,30 +1674,56 @@
       <c r="G16" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17" s="10"/>
-      <c r="B17" s="5" t="s">
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" t="s">
+        <v>78</v>
+      </c>
+      <c r="R16" t="s">
+        <v>78</v>
+      </c>
+      <c r="S16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A17" s="12"/>
+      <c r="B17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" s="8" t="s">
+      <c r="C17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" t="s">
+        <v>79</v>
+      </c>
+      <c r="R17" t="s">
+        <v>79</v>
+      </c>
+      <c r="S17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A19" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1110,72 +1744,124 @@
       <c r="G19" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A20" s="9"/>
-      <c r="B20" s="3" t="s">
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" t="s">
+        <v>80</v>
+      </c>
+      <c r="R19" t="s">
+        <v>80</v>
+      </c>
+      <c r="S19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A20" s="13"/>
+      <c r="B20" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A21" s="9"/>
-      <c r="B21" s="3" t="s">
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" t="s">
+        <v>84</v>
+      </c>
+      <c r="R20" t="s">
+        <v>81</v>
+      </c>
+      <c r="S20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A21" s="13"/>
+      <c r="B21" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A22" s="10"/>
-      <c r="B22" s="5" t="s">
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" t="s">
+        <v>85</v>
+      </c>
+      <c r="R21" t="s">
+        <v>82</v>
+      </c>
+      <c r="S21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A22" s="12"/>
+      <c r="B22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A24" s="8" t="s">
+      <c r="C22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" t="s">
+        <v>86</v>
+      </c>
+      <c r="R22" t="s">
+        <v>83</v>
+      </c>
+      <c r="S22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A24" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1196,72 +1882,120 @@
       <c r="G24" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A25" s="9"/>
-      <c r="B25" s="3" t="s">
+      <c r="L24" t="s">
+        <v>87</v>
+      </c>
+      <c r="M24" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="R24" t="s">
+        <v>97</v>
+      </c>
+      <c r="S24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A25" s="13"/>
+      <c r="B25" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="3" t="s">
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="3" t="s">
+      <c r="E25" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" t="s">
         <v>21</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="G25" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A26" s="9"/>
-      <c r="B26" s="3" t="s">
+      <c r="L25" t="s">
+        <v>88</v>
+      </c>
+      <c r="M25" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="R25" t="s">
+        <v>98</v>
+      </c>
+      <c r="S25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A26" s="13"/>
+      <c r="B26" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" s="3" t="s">
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" t="s">
         <v>24</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" s="3" t="s">
+      <c r="E26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" t="s">
         <v>21</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="G26" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A27" s="10"/>
-      <c r="B27" s="5" t="s">
+      <c r="L26" t="s">
+        <v>90</v>
+      </c>
+      <c r="M26" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="R26" t="s">
+        <v>99</v>
+      </c>
+      <c r="S26" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A27" s="12"/>
+      <c r="B27" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" s="5" t="s">
+      <c r="C27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E27" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" s="5" t="s">
+      <c r="E27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="G27" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A29" s="8" t="s">
+      <c r="L27" t="s">
+        <v>89</v>
+      </c>
+      <c r="M27" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="R27" t="s">
+        <v>100</v>
+      </c>
+      <c r="S27" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A29" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1282,30 +2016,54 @@
       <c r="G29" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A30" s="10"/>
-      <c r="B30" s="5" t="s">
+      <c r="L29" t="s">
+        <v>91</v>
+      </c>
+      <c r="M29" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="R29" t="s">
+        <v>101</v>
+      </c>
+      <c r="S29" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A30" s="12"/>
+      <c r="B30" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A32" s="8" t="s">
+      <c r="C30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L30" t="s">
+        <v>92</v>
+      </c>
+      <c r="M30" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="R30" t="s">
+        <v>102</v>
+      </c>
+      <c r="S30" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" ht="15.75" x14ac:dyDescent="0.45">
+      <c r="A32" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1326,86 +2084,122 @@
       <c r="G32" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A33" s="9"/>
-      <c r="B33" s="3" t="s">
+      <c r="L32" t="s">
+        <v>93</v>
+      </c>
+      <c r="R32" t="s">
+        <v>103</v>
+      </c>
+      <c r="S32" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" ht="15.75" x14ac:dyDescent="0.45">
+      <c r="A33" s="13"/>
+      <c r="B33" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D33" s="3" t="s">
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" t="s">
         <v>23</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A34" s="9"/>
-      <c r="B34" s="3" t="s">
+      <c r="E33" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" t="s">
+        <v>20</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L33" t="s">
+        <v>94</v>
+      </c>
+      <c r="R33" t="s">
+        <v>105</v>
+      </c>
+      <c r="S33" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" ht="15.75" x14ac:dyDescent="0.45">
+      <c r="A34" s="13"/>
+      <c r="B34" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D34" s="3" t="s">
+      <c r="C34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" t="s">
         <v>23</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A35" s="10"/>
-      <c r="B35" s="5" t="s">
+      <c r="E34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" t="s">
+        <v>20</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L34" t="s">
+        <v>95</v>
+      </c>
+      <c r="R34" t="s">
+        <v>104</v>
+      </c>
+      <c r="S34" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" ht="15.75" x14ac:dyDescent="0.45">
+      <c r="A35" s="12"/>
+      <c r="B35" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D35" s="5" t="s">
+      <c r="C35" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E35" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.45">
+      <c r="E35" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L35" t="s">
+        <v>96</v>
+      </c>
+      <c r="R35" t="s">
+        <v>106</v>
+      </c>
+      <c r="S35" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:19" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:19" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:19" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Add details for more AWS glue destination formats including hudi, parquet, and orc.
</commit_message>
<xml_diff>
--- a/aws_glue_s3_destination_file_properties.xlsx
+++ b/aws_glue_s3_destination_file_properties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earln\Documents\AWS\cloudnotes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E0CCC4-B104-4880-B198-85374E3C7C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773199E9-62D6-48E9-A96F-9C1A49375C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19670" yWindow="-21710" windowWidth="38620" windowHeight="21220" xr2:uid="{7AAB3D60-D17A-4906-8409-7A274DB37C5C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="130">
   <si>
     <t>CSV</t>
   </si>
@@ -430,15 +430,6 @@
     <t>pricingtrxcsvtoorcuncompressed</t>
   </si>
   <si>
-    <t>pricingtrxcsvtoparquetlzo</t>
-  </si>
-  <si>
-    <t>pricingtrxcsvtoparquetgzip</t>
-  </si>
-  <si>
-    <t>pricingtrxcsvtoparquetuncompressed</t>
-  </si>
-  <si>
     <t>pricingtrxhudigzip</t>
   </si>
   <si>
@@ -529,10 +520,52 @@
     <t>pricingtrxcsvtoiceberguncompressed.py</t>
   </si>
   <si>
-    <t>Hudi write op - insert; storage type = copy on write</t>
-  </si>
-  <si>
     <t>How to query delta lake when there this no glue table?</t>
+  </si>
+  <si>
+    <t>Avro with BZIP2 compression doesn't work. It is likely due to how AWS's script is compressing the file. Need to change to script to use native Spark libraries to write and compress the files.</t>
+  </si>
+  <si>
+    <t>Athena not working</t>
+  </si>
+  <si>
+    <t>Avro with GZIP compression doesn't work. It is likely due to how AWS's script is compressing the file. Need to change to script to use native Spark libraries to write and compress the files.</t>
+  </si>
+  <si>
+    <t>pricingtrxorcnone</t>
+  </si>
+  <si>
+    <t>pricingtrxavrogzip</t>
+  </si>
+  <si>
+    <t>pricingtrxavrobzip2</t>
+  </si>
+  <si>
+    <t>pricingtrxorcsnappy</t>
+  </si>
+  <si>
+    <t>pricingtrxparquetsnappy</t>
+  </si>
+  <si>
+    <t>pricingtrxparquetlzo</t>
+  </si>
+  <si>
+    <t>pricingtrxparquetgzip</t>
+  </si>
+  <si>
+    <t>pricingtrxparquetuncompressed</t>
+  </si>
+  <si>
+    <t>Doesn't create a Glue table. Created a crawler to manually crawl the S3 location. 3 min 22 sec to run crawler. Files have a snappy.orc suffix. This script includes "compression": "snappy", but that seems to be default even when the compression is none.</t>
+  </si>
+  <si>
+    <t>Doesn't create a Glue table. Created a crawler to manually crawl the S3 location. 3 min to run crawler. Files have a snappy.orc suffix. Seems to default to a snappy compression even when compression is set to none.</t>
+  </si>
+  <si>
+    <t>Small scanned data set and fast.</t>
+  </si>
+  <si>
+    <t>Hudi write op - insert; storage type = copy on write. Adds _hoodie_* fields to the table. .parquet file suffix</t>
   </si>
 </sst>
 </file>
@@ -541,7 +574,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -735,7 +768,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -749,6 +782,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -758,23 +804,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1092,8 +1122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F349F45-06DF-4A85-93CA-17D22A2819FA}">
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1106,9 +1136,11 @@
     <col min="6" max="6" width="23.1328125" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="26.53125" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="13.19921875" customWidth="1"/>
-    <col min="10" max="11" width="11.86328125" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.59765625" customWidth="1"/>
+    <col min="11" max="11" width="11.86328125" customWidth="1"/>
     <col min="12" max="12" width="33.1328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.1328125" style="20" customWidth="1"/>
+    <col min="13" max="13" width="33.1328125" style="12" customWidth="1"/>
     <col min="14" max="14" width="15.1328125" customWidth="1"/>
     <col min="15" max="15" width="12.06640625" customWidth="1"/>
     <col min="16" max="16" width="11.53125" customWidth="1"/>
@@ -1155,45 +1187,45 @@
       <c r="G3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="K3" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="L3" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="M3" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="N3" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="O3" s="15" t="s">
+      <c r="O3" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="P3" s="15" t="s">
+      <c r="P3" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="Q3" s="15" t="s">
+      <c r="Q3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="R3" s="15" t="s">
+      <c r="R3" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="S3" s="15" t="s">
+      <c r="S3" s="12" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="20" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
@@ -1214,22 +1246,22 @@
       <c r="G4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="13">
         <v>12182</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="13">
         <v>486906</v>
       </c>
-      <c r="J4" s="17">
+      <c r="J4" s="14">
         <v>46604041</v>
       </c>
-      <c r="K4" s="17">
+      <c r="K4" s="14">
         <v>3826</v>
       </c>
-      <c r="L4" s="17" t="s">
+      <c r="L4" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="M4" s="21"/>
+      <c r="M4" s="17"/>
       <c r="N4">
         <v>95</v>
       </c>
@@ -1239,7 +1271,7 @@
       <c r="P4">
         <v>44.45</v>
       </c>
-      <c r="Q4" s="19">
+      <c r="Q4" s="16">
         <v>9.0393518518518522E-3</v>
       </c>
       <c r="R4" t="s">
@@ -1250,7 +1282,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A5" s="13"/>
+      <c r="A5" s="20"/>
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -1269,13 +1301,13 @@
       <c r="G5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5" s="13">
         <v>12182</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="13">
         <v>486906</v>
       </c>
-      <c r="J5" s="17">
+      <c r="J5" s="14">
         <v>11850512</v>
       </c>
       <c r="K5">
@@ -1284,7 +1316,7 @@
       <c r="L5" t="s">
         <v>68</v>
       </c>
-      <c r="M5" s="20" t="s">
+      <c r="M5" s="12" t="s">
         <v>74</v>
       </c>
       <c r="N5">
@@ -1296,7 +1328,7 @@
       <c r="P5">
         <v>11.3</v>
       </c>
-      <c r="Q5" s="19">
+      <c r="Q5" s="16">
         <v>1.7222222222222222E-2</v>
       </c>
       <c r="R5" t="s">
@@ -1307,7 +1339,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A6" s="12"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
@@ -1326,13 +1358,13 @@
       <c r="G6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="16">
+      <c r="H6" s="13">
         <v>12182</v>
       </c>
-      <c r="I6" s="16">
+      <c r="I6" s="13">
         <v>486906</v>
       </c>
-      <c r="J6" s="17">
+      <c r="J6" s="14">
         <v>11999564</v>
       </c>
       <c r="K6">
@@ -1341,7 +1373,7 @@
       <c r="L6" t="s">
         <v>72</v>
       </c>
-      <c r="M6" s="20" t="s">
+      <c r="M6" s="12" t="s">
         <v>74</v>
       </c>
       <c r="N6">
@@ -1353,7 +1385,7 @@
       <c r="P6">
         <v>11.44</v>
       </c>
-      <c r="Q6" s="19">
+      <c r="Q6" s="16">
         <v>1.8067129629629631E-2</v>
       </c>
       <c r="R6" t="s">
@@ -1364,7 +1396,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1385,22 +1417,22 @@
       <c r="G8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="13">
         <v>12182</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="13">
         <v>486906</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J8" s="14">
         <v>135828163</v>
       </c>
-      <c r="K8" s="17">
+      <c r="K8" s="14">
         <v>11150</v>
       </c>
-      <c r="L8" s="17" t="s">
+      <c r="L8" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="M8" s="21"/>
+      <c r="M8" s="17"/>
       <c r="N8">
         <v>254</v>
       </c>
@@ -1410,7 +1442,7 @@
       <c r="P8">
         <v>129.54</v>
       </c>
-      <c r="Q8" s="18">
+      <c r="Q8" s="15">
         <v>1.8067129629629631E-2</v>
       </c>
       <c r="R8" t="s">
@@ -1421,7 +1453,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A9" s="13"/>
+      <c r="A9" s="20"/>
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -1440,16 +1472,16 @@
       <c r="G9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="22">
+      <c r="H9" s="13">
         <v>12182</v>
       </c>
-      <c r="I9" s="16">
+      <c r="I9" s="13">
         <v>486906</v>
       </c>
-      <c r="J9" s="17">
+      <c r="J9" s="14">
         <v>14345687</v>
       </c>
-      <c r="K9" s="17">
+      <c r="K9" s="14">
         <v>1178</v>
       </c>
       <c r="L9" t="s">
@@ -1464,7 +1496,7 @@
       <c r="P9">
         <v>13.68</v>
       </c>
-      <c r="Q9" s="19">
+      <c r="Q9" s="16">
         <v>1.7337962962962961E-2</v>
       </c>
       <c r="R9" t="s">
@@ -1475,7 +1507,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A10" s="12"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
@@ -1494,16 +1526,16 @@
       <c r="G10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="22">
+      <c r="H10" s="13">
         <v>12182</v>
       </c>
-      <c r="I10" s="16">
+      <c r="I10" s="13">
         <v>486906</v>
       </c>
-      <c r="J10" s="17">
+      <c r="J10" s="14">
         <v>13713152</v>
       </c>
-      <c r="K10" s="17">
+      <c r="K10" s="14">
         <v>1126</v>
       </c>
       <c r="L10" t="s">
@@ -1518,7 +1550,7 @@
       <c r="P10">
         <v>13.08</v>
       </c>
-      <c r="Q10" s="19">
+      <c r="Q10" s="16">
         <v>1.7754629629629631E-2</v>
       </c>
       <c r="R10" t="s">
@@ -1529,7 +1561,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="18" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1550,16 +1582,16 @@
       <c r="G12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="17">
+      <c r="H12" s="14">
         <v>12182</v>
       </c>
-      <c r="I12" s="17">
+      <c r="I12" s="14">
         <v>486906</v>
       </c>
-      <c r="J12" s="17">
+      <c r="J12" s="14">
         <v>62398096</v>
       </c>
-      <c r="K12" s="17">
+      <c r="K12" s="14">
         <v>5122</v>
       </c>
       <c r="L12" t="s">
@@ -1574,7 +1606,7 @@
       <c r="P12">
         <v>59.51</v>
       </c>
-      <c r="Q12" s="19">
+      <c r="Q12" s="16">
         <v>1.7222222222222222E-2</v>
       </c>
       <c r="R12" t="s">
@@ -1584,8 +1616,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A13" s="13"/>
+    <row r="13" spans="1:19" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A13" s="20"/>
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -1604,12 +1636,35 @@
       <c r="G13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
+      <c r="H13" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="J13" s="14">
+        <v>17308348</v>
+      </c>
+      <c r="K13" s="14">
+        <v>1421</v>
+      </c>
       <c r="L13" t="s">
-        <v>76</v>
+        <v>120</v>
+      </c>
+      <c r="M13" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="N13" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="O13" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="P13" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q13" s="16">
+        <v>1.7546296296296296E-2</v>
       </c>
       <c r="R13" t="s">
         <v>76</v>
@@ -1618,8 +1673,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A14" s="12"/>
+    <row r="14" spans="1:19" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A14" s="19"/>
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
@@ -1638,12 +1693,35 @@
       <c r="G14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
+      <c r="H14" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="J14" s="14">
+        <v>15468524</v>
+      </c>
+      <c r="K14" s="14">
+        <v>1270</v>
+      </c>
       <c r="L14" t="s">
-        <v>77</v>
+        <v>119</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="N14" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="O14" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="P14" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q14" s="16">
+        <v>1.8703703703703705E-2</v>
       </c>
       <c r="R14" t="s">
         <v>77</v>
@@ -1652,8 +1730,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A16" s="11" t="s">
+    <row r="16" spans="1:19" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A16" s="18" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1674,12 +1752,35 @@
       <c r="G16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
+      <c r="H16" s="14">
+        <v>12182</v>
+      </c>
+      <c r="I16" s="14">
+        <v>486906</v>
+      </c>
+      <c r="J16" s="14">
+        <v>36427740</v>
+      </c>
+      <c r="K16" s="14">
+        <v>2990</v>
+      </c>
       <c r="L16" t="s">
-        <v>78</v>
+        <v>118</v>
+      </c>
+      <c r="M16" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="N16">
+        <v>114</v>
+      </c>
+      <c r="O16">
+        <v>15.788</v>
+      </c>
+      <c r="P16">
+        <v>34.74</v>
+      </c>
+      <c r="Q16" s="16">
+        <v>1.7523148148148149E-2</v>
       </c>
       <c r="R16" t="s">
         <v>78</v>
@@ -1688,8 +1789,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A17" s="12"/>
+    <row r="17" spans="1:19" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A17" s="19"/>
       <c r="B17" s="4" t="s">
         <v>11</v>
       </c>
@@ -1708,12 +1809,35 @@
       <c r="G17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
+      <c r="H17" s="14">
+        <v>12182</v>
+      </c>
+      <c r="I17" s="14">
+        <v>486906</v>
+      </c>
+      <c r="J17" s="14">
+        <v>36427740</v>
+      </c>
+      <c r="K17" s="14">
+        <v>2990</v>
+      </c>
       <c r="L17" t="s">
-        <v>79</v>
+        <v>121</v>
+      </c>
+      <c r="M17" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="N17">
+        <v>109</v>
+      </c>
+      <c r="O17">
+        <v>16.835999999999999</v>
+      </c>
+      <c r="P17">
+        <v>34.74</v>
+      </c>
+      <c r="Q17" s="16">
+        <v>1.8414351851851852E-2</v>
       </c>
       <c r="R17" t="s">
         <v>79</v>
@@ -1723,7 +1847,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1744,12 +1868,35 @@
       <c r="G19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
+      <c r="H19" s="14">
+        <v>12182</v>
+      </c>
+      <c r="I19" s="14">
+        <v>486906</v>
+      </c>
+      <c r="J19" s="14">
+        <v>43928534</v>
+      </c>
+      <c r="K19" s="14">
+        <v>3606</v>
+      </c>
       <c r="L19" t="s">
-        <v>80</v>
+        <v>122</v>
+      </c>
+      <c r="M19" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="N19">
+        <v>120</v>
+      </c>
+      <c r="O19">
+        <v>14.196999999999999</v>
+      </c>
+      <c r="P19">
+        <v>5.99</v>
+      </c>
+      <c r="Q19" s="16">
+        <v>1.8263888888888889E-2</v>
       </c>
       <c r="R19" t="s">
         <v>80</v>
@@ -1759,7 +1906,7 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A20" s="13"/>
+      <c r="A20" s="20"/>
       <c r="B20" t="s">
         <v>12</v>
       </c>
@@ -1778,12 +1925,32 @@
       <c r="G20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
+      <c r="H20" s="14">
+        <v>12182</v>
+      </c>
+      <c r="I20" s="14">
+        <v>486906</v>
+      </c>
+      <c r="J20" s="14">
+        <v>43928534</v>
+      </c>
+      <c r="K20" s="14">
+        <v>3606</v>
+      </c>
       <c r="L20" t="s">
-        <v>84</v>
+        <v>123</v>
+      </c>
+      <c r="N20">
+        <v>118</v>
+      </c>
+      <c r="O20">
+        <v>15.595000000000001</v>
+      </c>
+      <c r="P20">
+        <v>5.99</v>
+      </c>
+      <c r="Q20" s="16">
+        <v>1.7627314814814814E-2</v>
       </c>
       <c r="R20" t="s">
         <v>81</v>
@@ -1793,7 +1960,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A21" s="13"/>
+      <c r="A21" s="20"/>
       <c r="B21" t="s">
         <v>9</v>
       </c>
@@ -1812,12 +1979,32 @@
       <c r="G21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
+      <c r="H21" s="14">
+        <v>12182</v>
+      </c>
+      <c r="I21" s="14">
+        <v>486906</v>
+      </c>
+      <c r="J21" s="14">
+        <v>43928534</v>
+      </c>
+      <c r="K21" s="14">
+        <v>3606</v>
+      </c>
       <c r="L21" t="s">
-        <v>85</v>
+        <v>124</v>
+      </c>
+      <c r="N21">
+        <v>127</v>
+      </c>
+      <c r="O21">
+        <v>15.702</v>
+      </c>
+      <c r="P21">
+        <v>5.99</v>
+      </c>
+      <c r="Q21" s="16">
+        <v>1.8379629629629628E-2</v>
       </c>
       <c r="R21" t="s">
         <v>82</v>
@@ -1827,7 +2014,7 @@
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A22" s="12"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="4" t="s">
         <v>13</v>
       </c>
@@ -1846,12 +2033,32 @@
       <c r="G22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
+      <c r="H22" s="14">
+        <v>12182</v>
+      </c>
+      <c r="I22" s="14">
+        <v>486906</v>
+      </c>
+      <c r="J22" s="14">
+        <v>43928534</v>
+      </c>
+      <c r="K22" s="14">
+        <v>3606</v>
+      </c>
       <c r="L22" t="s">
-        <v>86</v>
+        <v>125</v>
+      </c>
+      <c r="N22">
+        <v>111</v>
+      </c>
+      <c r="O22">
+        <v>13.228999999999999</v>
+      </c>
+      <c r="P22">
+        <v>5.99</v>
+      </c>
+      <c r="Q22" s="16">
+        <v>1.8078703703703704E-2</v>
       </c>
       <c r="R22" t="s">
         <v>83</v>
@@ -1860,8 +2067,8 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A24" s="11" t="s">
+    <row r="24" spans="1:19" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A24" s="18" t="s">
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -1882,21 +2089,45 @@
       <c r="G24" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="H24" s="21">
+        <v>12182</v>
+      </c>
+      <c r="I24" s="14">
+        <v>486906</v>
+      </c>
+      <c r="J24" s="14">
+        <v>5383451479</v>
+      </c>
+      <c r="K24" s="14">
+        <v>145526</v>
+      </c>
       <c r="L24" t="s">
-        <v>87</v>
-      </c>
-      <c r="M24" s="20" t="s">
-        <v>117</v>
+        <v>84</v>
+      </c>
+      <c r="M24" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="N24">
+        <v>103</v>
+      </c>
+      <c r="O24">
+        <v>44.600999999999999</v>
+      </c>
+      <c r="P24">
+        <v>6.18</v>
+      </c>
+      <c r="Q24" s="16">
+        <v>3.7743055555555557E-2</v>
       </c>
       <c r="R24" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="S24" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A25" s="13"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A25" s="20"/>
       <c r="B25" t="s">
         <v>12</v>
       </c>
@@ -1915,21 +2146,45 @@
       <c r="G25" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="H25" s="21">
+        <v>12182</v>
+      </c>
+      <c r="I25" s="14">
+        <v>486906</v>
+      </c>
+      <c r="J25" s="14">
+        <v>5385422479</v>
+      </c>
+      <c r="K25" s="14">
+        <v>145580</v>
+      </c>
       <c r="L25" t="s">
-        <v>88</v>
-      </c>
-      <c r="M25" s="20" t="s">
-        <v>117</v>
+        <v>85</v>
+      </c>
+      <c r="M25" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="N25" s="14">
+        <v>99</v>
+      </c>
+      <c r="O25">
+        <v>53.1</v>
+      </c>
+      <c r="P25">
+        <v>6.4</v>
+      </c>
+      <c r="Q25" s="16">
+        <v>3.7430555555555557E-2</v>
       </c>
       <c r="R25" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="S25" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A26" s="13"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A26" s="20"/>
       <c r="B26" t="s">
         <v>11</v>
       </c>
@@ -1948,21 +2203,45 @@
       <c r="G26" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="H26" s="21">
+        <v>12182</v>
+      </c>
+      <c r="I26" s="14">
+        <v>486906</v>
+      </c>
+      <c r="J26" s="14">
+        <v>5381617781</v>
+      </c>
+      <c r="K26" s="14">
+        <v>145477</v>
+      </c>
       <c r="L26" t="s">
-        <v>90</v>
-      </c>
-      <c r="M26" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="M26" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="N26">
         <v>117</v>
       </c>
+      <c r="O26">
+        <v>57.128999999999998</v>
+      </c>
+      <c r="P26">
+        <v>5.99</v>
+      </c>
+      <c r="Q26" s="16">
+        <v>3.9039351851851853E-2</v>
+      </c>
       <c r="R26" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="S26" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A27" s="12"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A27" s="19"/>
       <c r="B27" s="4" t="s">
         <v>13</v>
       </c>
@@ -1981,21 +2260,45 @@
       <c r="G27" s="5" t="s">
         <v>25</v>
       </c>
+      <c r="H27" s="21">
+        <v>12182</v>
+      </c>
+      <c r="I27" s="14">
+        <v>486906</v>
+      </c>
+      <c r="J27" s="14">
+        <v>5416476615</v>
+      </c>
+      <c r="K27" s="14">
+        <v>146419</v>
+      </c>
       <c r="L27" t="s">
-        <v>89</v>
-      </c>
-      <c r="M27" s="20" t="s">
-        <v>117</v>
+        <v>86</v>
+      </c>
+      <c r="M27" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="N27">
+        <v>106</v>
+      </c>
+      <c r="O27">
+        <v>45.325000000000003</v>
+      </c>
+      <c r="P27">
+        <v>7.5</v>
+      </c>
+      <c r="Q27" s="16">
+        <v>3.876157407407408E-2</v>
       </c>
       <c r="R27" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="S27" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="18" t="s">
         <v>6</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -2017,20 +2320,20 @@
         <v>20</v>
       </c>
       <c r="L29" t="s">
-        <v>91</v>
-      </c>
-      <c r="M29" s="20" t="s">
-        <v>118</v>
+        <v>88</v>
+      </c>
+      <c r="M29" s="12" t="s">
+        <v>114</v>
       </c>
       <c r="R29" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="S29" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A30" s="12"/>
+      <c r="A30" s="19"/>
       <c r="B30" s="4" t="s">
         <v>13</v>
       </c>
@@ -2050,20 +2353,20 @@
         <v>20</v>
       </c>
       <c r="L30" t="s">
-        <v>92</v>
-      </c>
-      <c r="M30" s="20" t="s">
-        <v>118</v>
+        <v>89</v>
+      </c>
+      <c r="M30" s="12" t="s">
+        <v>114</v>
       </c>
       <c r="R30" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="S30" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:19" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="18" t="s">
         <v>7</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -2085,17 +2388,17 @@
         <v>20</v>
       </c>
       <c r="L32" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="R32" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="S32" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:19" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A33" s="13"/>
+      <c r="A33" s="20"/>
       <c r="B33" t="s">
         <v>12</v>
       </c>
@@ -2115,17 +2418,17 @@
         <v>20</v>
       </c>
       <c r="L33" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="R33" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="S33" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:19" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A34" s="13"/>
+      <c r="A34" s="20"/>
       <c r="B34" t="s">
         <v>11</v>
       </c>
@@ -2145,17 +2448,17 @@
         <v>20</v>
       </c>
       <c r="L34" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="R34" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="S34" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:19" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A35" s="12"/>
+      <c r="A35" s="19"/>
       <c r="B35" s="4" t="s">
         <v>13</v>
       </c>
@@ -2175,13 +2478,13 @@
         <v>20</v>
       </c>
       <c r="L35" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="R35" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="S35" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:19" ht="15.75" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Add details for the deltalake file formats.
</commit_message>
<xml_diff>
--- a/aws_glue_s3_destination_file_properties.xlsx
+++ b/aws_glue_s3_destination_file_properties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earln\Documents\AWS\cloudnotes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773199E9-62D6-48E9-A96F-9C1A49375C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F5990B-D64D-4E24-A3FF-D350EFFFD303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19670" yWindow="-21710" windowWidth="38620" windowHeight="21220" xr2:uid="{7AAB3D60-D17A-4906-8409-7A274DB37C5C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="131">
   <si>
     <t>CSV</t>
   </si>
@@ -520,9 +520,6 @@
     <t>pricingtrxcsvtoiceberguncompressed.py</t>
   </si>
   <si>
-    <t>How to query delta lake when there this no glue table?</t>
-  </si>
-  <si>
     <t>Avro with BZIP2 compression doesn't work. It is likely due to how AWS's script is compressing the file. Need to change to script to use native Spark libraries to write and compress the files.</t>
   </si>
   <si>
@@ -566,6 +563,12 @@
   </si>
   <si>
     <t>Hudi write op - insert; storage type = copy on write. Adds _hoodie_* fields to the table. .parquet file suffix</t>
+  </si>
+  <si>
+    <t>Create a crawler and run it. Ran in 2:52 (mi:ss) File suffix snappy.parquet</t>
+  </si>
+  <si>
+    <t>Create a crawler and run it. Ran in 4:53 (mi:ss) File suffix snappy.parquet</t>
   </si>
 </sst>
 </file>
@@ -795,6 +798,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -804,7 +808,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1122,8 +1125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F349F45-06DF-4A85-93CA-17D22A2819FA}">
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView tabSelected="1" topLeftCell="B17" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1225,7 +1228,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
@@ -1282,7 +1285,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A5" s="20"/>
+      <c r="A5" s="21"/>
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -1339,7 +1342,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A6" s="19"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
@@ -1396,7 +1399,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1453,7 +1456,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A9" s="20"/>
+      <c r="A9" s="21"/>
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -1507,7 +1510,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A10" s="19"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
@@ -1561,7 +1564,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1617,7 +1620,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A13" s="20"/>
+      <c r="A13" s="21"/>
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -1637,10 +1640,10 @@
         <v>20</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J13" s="14">
         <v>17308348</v>
@@ -1649,19 +1652,19 @@
         <v>1421</v>
       </c>
       <c r="L13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M13" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="N13" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="N13" s="14" t="s">
-        <v>116</v>
-      </c>
       <c r="O13" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P13" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q13" s="16">
         <v>1.7546296296296296E-2</v>
@@ -1674,7 +1677,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A14" s="19"/>
+      <c r="A14" s="20"/>
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
@@ -1694,10 +1697,10 @@
         <v>20</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J14" s="14">
         <v>15468524</v>
@@ -1706,19 +1709,19 @@
         <v>1270</v>
       </c>
       <c r="L14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M14" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N14" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O14" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P14" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q14" s="16">
         <v>1.8703703703703705E-2</v>
@@ -1731,7 +1734,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1765,10 +1768,10 @@
         <v>2990</v>
       </c>
       <c r="L16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M16" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N16">
         <v>114</v>
@@ -1790,7 +1793,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A17" s="19"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="4" t="s">
         <v>11</v>
       </c>
@@ -1822,10 +1825,10 @@
         <v>2990</v>
       </c>
       <c r="L17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M17" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N17">
         <v>109</v>
@@ -1847,7 +1850,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="19" t="s">
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1881,10 +1884,10 @@
         <v>3606</v>
       </c>
       <c r="L19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M19" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N19">
         <v>120</v>
@@ -1906,7 +1909,7 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A20" s="20"/>
+      <c r="A20" s="21"/>
       <c r="B20" t="s">
         <v>12</v>
       </c>
@@ -1938,7 +1941,7 @@
         <v>3606</v>
       </c>
       <c r="L20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N20">
         <v>118</v>
@@ -1960,7 +1963,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A21" s="20"/>
+      <c r="A21" s="21"/>
       <c r="B21" t="s">
         <v>9</v>
       </c>
@@ -1992,7 +1995,7 @@
         <v>3606</v>
       </c>
       <c r="L21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N21">
         <v>127</v>
@@ -2014,7 +2017,7 @@
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A22" s="19"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="4" t="s">
         <v>13</v>
       </c>
@@ -2046,7 +2049,7 @@
         <v>3606</v>
       </c>
       <c r="L22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N22">
         <v>111</v>
@@ -2068,7 +2071,7 @@
       </c>
     </row>
     <row r="24" spans="1:19" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="19" t="s">
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -2089,7 +2092,7 @@
       <c r="G24" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H24" s="21">
+      <c r="H24" s="18">
         <v>12182</v>
       </c>
       <c r="I24" s="14">
@@ -2105,7 +2108,7 @@
         <v>84</v>
       </c>
       <c r="M24" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N24">
         <v>103</v>
@@ -2127,7 +2130,7 @@
       </c>
     </row>
     <row r="25" spans="1:19" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A25" s="20"/>
+      <c r="A25" s="21"/>
       <c r="B25" t="s">
         <v>12</v>
       </c>
@@ -2146,7 +2149,7 @@
       <c r="G25" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H25" s="21">
+      <c r="H25" s="18">
         <v>12182</v>
       </c>
       <c r="I25" s="14">
@@ -2162,7 +2165,7 @@
         <v>85</v>
       </c>
       <c r="M25" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N25" s="14">
         <v>99</v>
@@ -2184,7 +2187,7 @@
       </c>
     </row>
     <row r="26" spans="1:19" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A26" s="20"/>
+      <c r="A26" s="21"/>
       <c r="B26" t="s">
         <v>11</v>
       </c>
@@ -2203,7 +2206,7 @@
       <c r="G26" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H26" s="21">
+      <c r="H26" s="18">
         <v>12182</v>
       </c>
       <c r="I26" s="14">
@@ -2219,7 +2222,7 @@
         <v>87</v>
       </c>
       <c r="M26" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N26">
         <v>117</v>
@@ -2241,7 +2244,7 @@
       </c>
     </row>
     <row r="27" spans="1:19" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A27" s="19"/>
+      <c r="A27" s="20"/>
       <c r="B27" s="4" t="s">
         <v>13</v>
       </c>
@@ -2260,7 +2263,7 @@
       <c r="G27" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H27" s="21">
+      <c r="H27" s="18">
         <v>12182</v>
       </c>
       <c r="I27" s="14">
@@ -2276,7 +2279,7 @@
         <v>86</v>
       </c>
       <c r="M27" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N27">
         <v>106</v>
@@ -2298,7 +2301,7 @@
       </c>
     </row>
     <row r="29" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -2319,11 +2322,35 @@
       <c r="G29" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="H29" s="18">
+        <v>12182</v>
+      </c>
+      <c r="I29" s="14">
+        <v>486906</v>
+      </c>
+      <c r="J29" s="14">
+        <v>58828879</v>
+      </c>
+      <c r="K29" s="14">
+        <v>4828</v>
+      </c>
       <c r="L29" t="s">
         <v>88</v>
       </c>
       <c r="M29" s="12" t="s">
-        <v>114</v>
+        <v>129</v>
+      </c>
+      <c r="N29">
+        <v>91</v>
+      </c>
+      <c r="O29">
+        <v>13.36</v>
+      </c>
+      <c r="P29">
+        <v>5.99</v>
+      </c>
+      <c r="Q29" s="16">
+        <v>1.7523148148148149E-2</v>
       </c>
       <c r="R29" t="s">
         <v>98</v>
@@ -2333,7 +2360,7 @@
       </c>
     </row>
     <row r="30" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A30" s="19"/>
+      <c r="A30" s="20"/>
       <c r="B30" s="4" t="s">
         <v>13</v>
       </c>
@@ -2352,11 +2379,35 @@
       <c r="G30" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="H30" s="18">
+        <v>12182</v>
+      </c>
+      <c r="I30" s="14">
+        <v>486906</v>
+      </c>
+      <c r="J30" s="14">
+        <v>58828879</v>
+      </c>
+      <c r="K30" s="14">
+        <v>4828</v>
+      </c>
       <c r="L30" t="s">
         <v>89</v>
       </c>
       <c r="M30" s="12" t="s">
-        <v>114</v>
+        <v>130</v>
+      </c>
+      <c r="N30">
+        <v>122</v>
+      </c>
+      <c r="O30">
+        <v>19.73</v>
+      </c>
+      <c r="P30">
+        <v>5.99</v>
+      </c>
+      <c r="Q30" s="16">
+        <v>1.6689814814814817E-2</v>
       </c>
       <c r="R30" t="s">
         <v>99</v>
@@ -2366,7 +2417,7 @@
       </c>
     </row>
     <row r="32" spans="1:19" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -2398,7 +2449,7 @@
       </c>
     </row>
     <row r="33" spans="1:19" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A33" s="20"/>
+      <c r="A33" s="21"/>
       <c r="B33" t="s">
         <v>12</v>
       </c>
@@ -2428,7 +2479,7 @@
       </c>
     </row>
     <row r="34" spans="1:19" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A34" s="20"/>
+      <c r="A34" s="21"/>
       <c r="B34" t="s">
         <v>11</v>
       </c>
@@ -2458,7 +2509,7 @@
       </c>
     </row>
     <row r="35" spans="1:19" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A35" s="19"/>
+      <c r="A35" s="20"/>
       <c r="B35" s="4" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Finish metrics for the iceberg formats.
</commit_message>
<xml_diff>
--- a/aws_glue_s3_destination_file_properties.xlsx
+++ b/aws_glue_s3_destination_file_properties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earln\Documents\AWS\cloudnotes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F5990B-D64D-4E24-A3FF-D350EFFFD303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2B18E5-0B0B-4D0D-B7EF-8F71D9C9D12A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19670" yWindow="-21710" windowWidth="38620" windowHeight="21220" xr2:uid="{7AAB3D60-D17A-4906-8409-7A274DB37C5C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="135">
   <si>
     <t>CSV</t>
   </si>
@@ -569,6 +569,18 @@
   </si>
   <si>
     <t>Create a crawler and run it. Ran in 4:53 (mi:ss) File suffix snappy.parquet</t>
+  </si>
+  <si>
+    <t>Fastest scan and smallest data size scanned. Puts all files in one S3 prefix s3://pricingtrxprocessed/iceberggzip/pricingtrx/pricingtrxiceberggzip/data/. Has a metadata prefix with 3 files. Files have .parquet suffix.</t>
+  </si>
+  <si>
+    <t>Fastest scan and smallest data size scanned. Puts all files in one S3 prefix s3://pricingtrxprocessed/iceberggzip/pricingtrx/pricingtrxiceberglzo/data/. Has a metadata prefix with 3 files. Files have .parquet suffix.</t>
+  </si>
+  <si>
+    <t>Fastest scan and smallest data size scanned. Puts all files in one S3 prefix s3://pricingtrxprocessed/iceberggzip/pricingtrx/pricingtrxicebergsnappy/data/. Has a metadata prefix with 3 files. Files have .parquet suffix.</t>
+  </si>
+  <si>
+    <t>Fastest scan and smallest data size scanned. Puts all files in one S3 prefix s3://pricingtrxprocessed/iceberggzip/pricingtrx/pricingtrxiceberguncompressed/data/. Has a metadata prefix with 3 files. Files have .parquet suffix.</t>
   </si>
 </sst>
 </file>
@@ -1125,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F349F45-06DF-4A85-93CA-17D22A2819FA}">
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2416,7 +2428,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:19" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A32" s="19" t="s">
         <v>7</v>
       </c>
@@ -2438,9 +2450,36 @@
       <c r="G32" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="H32" s="18">
+        <v>12182</v>
+      </c>
+      <c r="I32" s="14">
+        <v>486906</v>
+      </c>
+      <c r="J32" s="14">
+        <v>73453103</v>
+      </c>
+      <c r="K32" s="14">
+        <v>6028</v>
+      </c>
       <c r="L32" t="s">
         <v>90</v>
       </c>
+      <c r="M32" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="N32">
+        <v>119</v>
+      </c>
+      <c r="O32">
+        <v>3.35</v>
+      </c>
+      <c r="P32">
+        <v>4.97</v>
+      </c>
+      <c r="Q32" s="16">
+        <v>1.8935185185185183E-2</v>
+      </c>
       <c r="R32" t="s">
         <v>100</v>
       </c>
@@ -2448,7 +2487,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:19" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A33" s="21"/>
       <c r="B33" t="s">
         <v>12</v>
@@ -2468,9 +2507,36 @@
       <c r="G33" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="H33" s="18">
+        <v>12182</v>
+      </c>
+      <c r="I33" s="14">
+        <v>486906</v>
+      </c>
+      <c r="J33" s="14">
+        <v>73452937</v>
+      </c>
+      <c r="K33" s="14">
+        <v>6028</v>
+      </c>
       <c r="L33" t="s">
         <v>91</v>
       </c>
+      <c r="M33" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="N33" s="14">
+        <v>111</v>
+      </c>
+      <c r="O33">
+        <v>9.3360000000000003</v>
+      </c>
+      <c r="P33">
+        <v>4.97</v>
+      </c>
+      <c r="Q33" s="16">
+        <v>1.8472222222222223E-2</v>
+      </c>
       <c r="R33" t="s">
         <v>102</v>
       </c>
@@ -2478,7 +2544,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:19" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A34" s="21"/>
       <c r="B34" t="s">
         <v>11</v>
@@ -2498,9 +2564,36 @@
       <c r="G34" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="H34" s="18">
+        <v>12182</v>
+      </c>
+      <c r="I34" s="14">
+        <v>486906</v>
+      </c>
+      <c r="J34" s="14">
+        <v>73454861</v>
+      </c>
+      <c r="K34" s="14">
+        <v>6028</v>
+      </c>
       <c r="L34" t="s">
         <v>92</v>
       </c>
+      <c r="M34" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="N34">
+        <v>106</v>
+      </c>
+      <c r="O34">
+        <v>6.1470000000000002</v>
+      </c>
+      <c r="P34">
+        <v>4.97</v>
+      </c>
+      <c r="Q34" s="16">
+        <v>1.834490740740741E-2</v>
+      </c>
       <c r="R34" t="s">
         <v>101</v>
       </c>
@@ -2508,7 +2601,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="15.75" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:19" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A35" s="20"/>
       <c r="B35" s="4" t="s">
         <v>13</v>
@@ -2528,8 +2621,35 @@
       <c r="G35" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="H35" s="18">
+        <v>12182</v>
+      </c>
+      <c r="I35" s="14">
+        <v>486906</v>
+      </c>
+      <c r="J35" s="14">
+        <v>73458508</v>
+      </c>
+      <c r="K35" s="14">
+        <v>6028</v>
+      </c>
       <c r="L35" t="s">
         <v>93</v>
+      </c>
+      <c r="M35" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="N35" s="14">
+        <v>114</v>
+      </c>
+      <c r="O35" s="14">
+        <v>5.6219999999999999</v>
+      </c>
+      <c r="P35">
+        <v>4.97</v>
+      </c>
+      <c r="Q35" s="16">
+        <v>1.7465277777777777E-2</v>
       </c>
       <c r="R35" t="s">
         <v>103</v>

</xml_diff>

<commit_message>
Cleaned up the xlsx file and improved the readme.md.
</commit_message>
<xml_diff>
--- a/aws_glue_s3_destination_file_properties.xlsx
+++ b/aws_glue_s3_destination_file_properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earln\Documents\AWS\cloudnotes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2B18E5-0B0B-4D0D-B7EF-8F71D9C9D12A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F45A99-C071-4E10-99A7-A1F4FF99C11F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19670" yWindow="-21710" windowWidth="38620" windowHeight="21220" xr2:uid="{7AAB3D60-D17A-4906-8409-7A274DB37C5C}"/>
+    <workbookView xWindow="-23360" yWindow="-21790" windowWidth="38620" windowHeight="21220" xr2:uid="{7AAB3D60-D17A-4906-8409-7A274DB37C5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="135">
   <si>
     <t>CSV</t>
   </si>
@@ -520,15 +520,9 @@
     <t>pricingtrxcsvtoiceberguncompressed.py</t>
   </si>
   <si>
-    <t>Avro with BZIP2 compression doesn't work. It is likely due to how AWS's script is compressing the file. Need to change to script to use native Spark libraries to write and compress the files.</t>
-  </si>
-  <si>
     <t>Athena not working</t>
   </si>
   <si>
-    <t>Avro with GZIP compression doesn't work. It is likely due to how AWS's script is compressing the file. Need to change to script to use native Spark libraries to write and compress the files.</t>
-  </si>
-  <si>
     <t>pricingtrxorcnone</t>
   </si>
   <si>
@@ -581,6 +575,12 @@
   </si>
   <si>
     <t>Fastest scan and smallest data size scanned. Puts all files in one S3 prefix s3://pricingtrxprocessed/iceberggzip/pricingtrx/pricingtrxiceberguncompressed/data/. Has a metadata prefix with 3 files. Files have .parquet suffix.</t>
+  </si>
+  <si>
+    <t>Avro with BZIP2 compression doesn't work. It is likely due to how AWS's script is compressing the file. Need to change the script to use native Spark libraries to write and compress the files.</t>
+  </si>
+  <si>
+    <t>Athena Query Results</t>
   </si>
 </sst>
 </file>
@@ -591,7 +591,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -621,16 +621,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -640,38 +654,179 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -681,45 +836,36 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -728,54 +874,43 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -783,41 +918,78 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -839,9 +1011,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -879,7 +1051,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -985,7 +1157,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1127,7 +1299,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1137,35 +1309,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F349F45-06DF-4A85-93CA-17D22A2819FA}">
   <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="15.1328125" customWidth="1"/>
-    <col min="2" max="2" width="19.3984375" customWidth="1"/>
+    <col min="2" max="2" width="13.53125" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="15" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="12.796875" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="23.1328125" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="26.53125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="13.19921875" customWidth="1"/>
-    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="9.9296875" customWidth="1"/>
     <col min="10" max="10" width="14.59765625" customWidth="1"/>
     <col min="11" max="11" width="11.86328125" customWidth="1"/>
     <col min="12" max="12" width="33.1328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.1328125" style="12" customWidth="1"/>
+    <col min="13" max="13" width="33.1328125" style="3" customWidth="1"/>
     <col min="14" max="14" width="15.1328125" customWidth="1"/>
     <col min="15" max="15" width="12.06640625" customWidth="1"/>
-    <col min="16" max="16" width="11.53125" customWidth="1"/>
+    <col min="16" max="16" width="12.796875" customWidth="1"/>
     <col min="17" max="17" width="12.53125" customWidth="1"/>
     <col min="18" max="18" width="41.796875" customWidth="1"/>
     <col min="19" max="19" width="46.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.65">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:19" ht="21.4" thickBot="1" x14ac:dyDescent="0.7">
+      <c r="A1" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1176,186 +1348,192 @@
       <c r="J2" t="s">
         <v>42</v>
       </c>
-      <c r="N2" t="s">
+      <c r="L2" t="s">
         <v>43</v>
       </c>
+      <c r="N2" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="33"/>
     </row>
     <row r="3" spans="1:19" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="M3" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="N3" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="O3" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="P3" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="Q3" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="R3" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="S3" s="12" t="s">
+      <c r="S3" s="30" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="C4" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="13">
+      <c r="F4" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="23">
         <v>12182</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4" s="23">
         <v>486906</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="24">
         <v>46604041</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="24">
         <v>3826</v>
       </c>
-      <c r="L4" s="14" t="s">
+      <c r="L4" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="M4" s="17"/>
-      <c r="N4">
+      <c r="M4" s="25"/>
+      <c r="N4" s="22">
         <v>95</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="22">
         <v>14.218</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="22">
         <v>44.45</v>
       </c>
-      <c r="Q4" s="16">
+      <c r="Q4" s="26">
         <v>9.0393518518518522E-3</v>
       </c>
-      <c r="R4" t="s">
+      <c r="R4" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="S4" t="s">
+      <c r="S4" s="27" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A5" s="21"/>
-      <c r="B5" t="s">
+      <c r="A5" s="40"/>
+      <c r="B5" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="C5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="13">
+      <c r="F5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="6">
         <v>12182</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="6">
         <v>486906</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="7">
         <v>11850512</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="4">
         <v>973</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="M5" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="4">
         <v>99</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="4">
         <v>15.488</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="4">
         <v>11.3</v>
       </c>
-      <c r="Q5" s="16">
+      <c r="Q5" s="9">
         <v>1.7222222222222222E-2</v>
       </c>
-      <c r="R5" t="s">
+      <c r="R5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="S5" t="s">
+      <c r="S5" s="14" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A6" s="20"/>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="40"/>
+      <c r="B6" s="35" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1370,160 +1548,182 @@
       <c r="F6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="13">
+      <c r="G6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="6">
         <v>12182</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="6">
         <v>486906</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="7">
         <v>11999564</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="4">
         <v>985</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="M6" s="12" t="s">
+      <c r="M6" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="4">
         <v>118</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="4">
         <v>15.792999999999999</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="4">
         <v>11.44</v>
       </c>
-      <c r="Q6" s="16">
+      <c r="Q6" s="9">
         <v>1.8067129629629631E-2</v>
       </c>
-      <c r="R6" t="s">
+      <c r="R6" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="S6" t="s">
+      <c r="S6" s="14" t="s">
         <v>52</v>
       </c>
     </row>
+    <row r="7" spans="1:19" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="41"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="15"/>
+    </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="C8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="13">
+      <c r="F8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="6">
         <v>12182</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="6">
         <v>486906</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="7">
         <v>135828163</v>
       </c>
-      <c r="K8" s="14">
+      <c r="K8" s="7">
         <v>11150</v>
       </c>
-      <c r="L8" s="14" t="s">
+      <c r="L8" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="M8" s="17"/>
-      <c r="N8">
+      <c r="M8" s="8"/>
+      <c r="N8" s="4">
         <v>254</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="4">
         <v>21.884</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="4">
         <v>129.54</v>
       </c>
-      <c r="Q8" s="15">
+      <c r="Q8" s="10">
         <v>1.8067129629629631E-2</v>
       </c>
-      <c r="R8" t="s">
+      <c r="R8" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="S8" t="s">
+      <c r="S8" s="14" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A9" s="21"/>
-      <c r="B9" t="s">
+      <c r="A9" s="40"/>
+      <c r="B9" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="C9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="13">
+      <c r="F9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="6">
         <v>12182</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="6">
         <v>486906</v>
       </c>
-      <c r="J9" s="14">
+      <c r="J9" s="7">
         <v>14345687</v>
       </c>
-      <c r="K9" s="14">
+      <c r="K9" s="7">
         <v>1178</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="N9">
+      <c r="M9" s="5"/>
+      <c r="N9" s="4">
         <v>105</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="4">
         <v>15.090999999999999</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="4">
         <v>13.68</v>
       </c>
-      <c r="Q9" s="16">
+      <c r="Q9" s="9">
         <v>1.7337962962962961E-2</v>
       </c>
-      <c r="R9" t="s">
+      <c r="R9" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="S9" t="s">
+      <c r="S9" s="14" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A10" s="20"/>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="40"/>
+      <c r="B10" s="35" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -1538,159 +1738,182 @@
       <c r="F10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="13">
+      <c r="G10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="6">
         <v>12182</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="6">
         <v>486906</v>
       </c>
-      <c r="J10" s="14">
+      <c r="J10" s="7">
         <v>13713152</v>
       </c>
-      <c r="K10" s="14">
+      <c r="K10" s="7">
         <v>1126</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="N10">
+      <c r="M10" s="5"/>
+      <c r="N10" s="4">
         <v>118</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="4">
         <v>17.366</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="4">
         <v>13.08</v>
       </c>
-      <c r="Q10" s="16">
+      <c r="Q10" s="9">
         <v>1.7754629629629631E-2</v>
       </c>
-      <c r="R10" t="s">
+      <c r="R10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="S10" t="s">
+      <c r="S10" s="14" t="s">
         <v>56</v>
       </c>
     </row>
+    <row r="11" spans="1:19" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="41"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="15"/>
+    </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="C12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="14">
+      <c r="F12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="7">
         <v>12182</v>
       </c>
-      <c r="I12" s="14">
+      <c r="I12" s="7">
         <v>486906</v>
       </c>
-      <c r="J12" s="14">
+      <c r="J12" s="7">
         <v>62398096</v>
       </c>
-      <c r="K12" s="14">
+      <c r="K12" s="7">
         <v>5122</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="N12">
+      <c r="M12" s="5"/>
+      <c r="N12" s="4">
         <v>100</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="4">
         <v>14.818</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="4">
         <v>59.51</v>
       </c>
-      <c r="Q12" s="16">
+      <c r="Q12" s="9">
         <v>1.7222222222222222E-2</v>
       </c>
-      <c r="R12" t="s">
+      <c r="R12" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="S12" t="s">
+      <c r="S12" s="14" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A13" s="21"/>
-      <c r="B13" t="s">
+      <c r="A13" s="40"/>
+      <c r="B13" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="C13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="J13" s="14">
+      <c r="F13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="J13" s="7">
         <v>17308348</v>
       </c>
-      <c r="K13" s="14">
+      <c r="K13" s="7">
         <v>1421</v>
       </c>
-      <c r="L13" t="s">
-        <v>119</v>
-      </c>
-      <c r="M13" s="12" t="s">
+      <c r="L13" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="N13" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="N13" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="O13" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="P13" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q13" s="16">
+      <c r="O13" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="P13" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q13" s="9">
         <v>1.7546296296296296E-2</v>
       </c>
-      <c r="R13" t="s">
+      <c r="R13" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="S13" t="s">
+      <c r="S13" s="14" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A14" s="20"/>
-      <c r="B14" s="4" t="s">
+      <c r="A14" s="40"/>
+      <c r="B14" s="35" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -1705,108 +1928,129 @@
       <c r="F14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="14" t="s">
+      <c r="G14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="J14" s="7">
+        <v>15468524</v>
+      </c>
+      <c r="K14" s="7">
+        <v>1270</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="M14" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="O14" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="P14" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q14" s="9">
+        <v>1.8703703703703705E-2</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="S14" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="41"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="15"/>
+    </row>
+    <row r="16" spans="1:19" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A16" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="7">
+        <v>12182</v>
+      </c>
+      <c r="I16" s="7">
+        <v>486906</v>
+      </c>
+      <c r="J16" s="7">
+        <v>36427740</v>
+      </c>
+      <c r="K16" s="7">
+        <v>2990</v>
+      </c>
+      <c r="L16" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="I14" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="J14" s="14">
-        <v>15468524</v>
-      </c>
-      <c r="K14" s="14">
-        <v>1270</v>
-      </c>
-      <c r="L14" t="s">
-        <v>118</v>
-      </c>
-      <c r="M14" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="N14" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="O14" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="P14" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q14" s="16">
-        <v>1.8703703703703705E-2</v>
-      </c>
-      <c r="R14" t="s">
-        <v>77</v>
-      </c>
-      <c r="S14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A16" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H16" s="14">
-        <v>12182</v>
-      </c>
-      <c r="I16" s="14">
-        <v>486906</v>
-      </c>
-      <c r="J16" s="14">
-        <v>36427740</v>
-      </c>
-      <c r="K16" s="14">
-        <v>2990</v>
-      </c>
-      <c r="L16" t="s">
-        <v>117</v>
-      </c>
-      <c r="M16" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="N16">
+      <c r="M16" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="N16" s="4">
         <v>114</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="4">
         <v>15.788</v>
       </c>
-      <c r="P16">
+      <c r="P16" s="4">
         <v>34.74</v>
       </c>
-      <c r="Q16" s="16">
+      <c r="Q16" s="9">
         <v>1.7523148148148149E-2</v>
       </c>
-      <c r="R16" t="s">
+      <c r="R16" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="S16" t="s">
+      <c r="S16" s="14" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A17" s="20"/>
-      <c r="B17" s="4" t="s">
+      <c r="A17" s="40"/>
+      <c r="B17" s="35" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -1821,216 +2065,243 @@
       <c r="F17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H17" s="14">
+      <c r="G17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="7">
         <v>12182</v>
       </c>
-      <c r="I17" s="14">
+      <c r="I17" s="7">
         <v>486906</v>
       </c>
-      <c r="J17" s="14">
+      <c r="J17" s="7">
         <v>36427740</v>
       </c>
-      <c r="K17" s="14">
+      <c r="K17" s="7">
         <v>2990</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L17" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="N17" s="4">
+        <v>109</v>
+      </c>
+      <c r="O17" s="4">
+        <v>16.835999999999999</v>
+      </c>
+      <c r="P17" s="4">
+        <v>34.74</v>
+      </c>
+      <c r="Q17" s="9">
+        <v>1.8414351851851852E-2</v>
+      </c>
+      <c r="R17" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="S17" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="41"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="15"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A19" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="7">
+        <v>12182</v>
+      </c>
+      <c r="I19" s="7">
+        <v>486906</v>
+      </c>
+      <c r="J19" s="7">
+        <v>43928534</v>
+      </c>
+      <c r="K19" s="7">
+        <v>3606</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="N19" s="4">
         <v>120</v>
       </c>
-      <c r="M17" s="12" t="s">
+      <c r="O19" s="4">
+        <v>14.196999999999999</v>
+      </c>
+      <c r="P19" s="4">
+        <v>5.99</v>
+      </c>
+      <c r="Q19" s="9">
+        <v>1.8263888888888889E-2</v>
+      </c>
+      <c r="R19" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="S19" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A20" s="40"/>
+      <c r="B20" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="7">
+        <v>12182</v>
+      </c>
+      <c r="I20" s="7">
+        <v>486906</v>
+      </c>
+      <c r="J20" s="7">
+        <v>43928534</v>
+      </c>
+      <c r="K20" s="7">
+        <v>3606</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="M20" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="N17">
-        <v>109</v>
-      </c>
-      <c r="O17">
-        <v>16.835999999999999</v>
-      </c>
-      <c r="P17">
-        <v>34.74</v>
-      </c>
-      <c r="Q17" s="16">
-        <v>1.8414351851851852E-2</v>
-      </c>
-      <c r="R17" t="s">
-        <v>79</v>
-      </c>
-      <c r="S17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A19" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="N20" s="4">
+        <v>118</v>
+      </c>
+      <c r="O20" s="4">
+        <v>15.595000000000001</v>
+      </c>
+      <c r="P20" s="4">
+        <v>5.99</v>
+      </c>
+      <c r="Q20" s="9">
+        <v>1.7627314814814814E-2</v>
+      </c>
+      <c r="R20" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="S20" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A21" s="40"/>
+      <c r="B21" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="14">
+      <c r="F21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="7">
         <v>12182</v>
       </c>
-      <c r="I19" s="14">
+      <c r="I21" s="7">
         <v>486906</v>
       </c>
-      <c r="J19" s="14">
+      <c r="J21" s="7">
         <v>43928534</v>
       </c>
-      <c r="K19" s="14">
+      <c r="K21" s="7">
         <v>3606</v>
       </c>
-      <c r="L19" t="s">
+      <c r="L21" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="M19" s="12" t="s">
+      <c r="M21" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="N21" s="4">
         <v>127</v>
       </c>
-      <c r="N19">
-        <v>120</v>
-      </c>
-      <c r="O19">
-        <v>14.196999999999999</v>
-      </c>
-      <c r="P19">
+      <c r="O21" s="4">
+        <v>15.702</v>
+      </c>
+      <c r="P21" s="4">
         <v>5.99</v>
       </c>
-      <c r="Q19" s="16">
-        <v>1.8263888888888889E-2</v>
-      </c>
-      <c r="R19" t="s">
-        <v>80</v>
-      </c>
-      <c r="S19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A20" s="21"/>
-      <c r="B20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" t="s">
-        <v>20</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="14">
-        <v>12182</v>
-      </c>
-      <c r="I20" s="14">
-        <v>486906</v>
-      </c>
-      <c r="J20" s="14">
-        <v>43928534</v>
-      </c>
-      <c r="K20" s="14">
-        <v>3606</v>
-      </c>
-      <c r="L20" t="s">
-        <v>122</v>
-      </c>
-      <c r="N20">
-        <v>118</v>
-      </c>
-      <c r="O20">
-        <v>15.595000000000001</v>
-      </c>
-      <c r="P20">
-        <v>5.99</v>
-      </c>
-      <c r="Q20" s="16">
-        <v>1.7627314814814814E-2</v>
-      </c>
-      <c r="R20" t="s">
-        <v>81</v>
-      </c>
-      <c r="S20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A21" s="21"/>
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H21" s="14">
-        <v>12182</v>
-      </c>
-      <c r="I21" s="14">
-        <v>486906</v>
-      </c>
-      <c r="J21" s="14">
-        <v>43928534</v>
-      </c>
-      <c r="K21" s="14">
-        <v>3606</v>
-      </c>
-      <c r="L21" t="s">
-        <v>123</v>
-      </c>
-      <c r="N21">
-        <v>127</v>
-      </c>
-      <c r="O21">
-        <v>15.702</v>
-      </c>
-      <c r="P21">
-        <v>5.99</v>
-      </c>
-      <c r="Q21" s="16">
+      <c r="Q21" s="9">
         <v>1.8379629629629628E-2</v>
       </c>
-      <c r="R21" t="s">
+      <c r="R21" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="S21" t="s">
+      <c r="S21" s="14" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A22" s="20"/>
-      <c r="B22" s="4" t="s">
+      <c r="A22" s="40"/>
+      <c r="B22" s="35" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -2045,219 +2316,243 @@
       <c r="F22" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G22" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22" s="14">
+      <c r="G22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="7">
         <v>12182</v>
       </c>
-      <c r="I22" s="14">
+      <c r="I22" s="7">
         <v>486906</v>
       </c>
-      <c r="J22" s="14">
+      <c r="J22" s="7">
         <v>43928534</v>
       </c>
-      <c r="K22" s="14">
+      <c r="K22" s="7">
         <v>3606</v>
       </c>
-      <c r="L22" t="s">
-        <v>124</v>
-      </c>
-      <c r="N22">
+      <c r="L22" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="N22" s="4">
         <v>111</v>
       </c>
-      <c r="O22">
+      <c r="O22" s="4">
         <v>13.228999999999999</v>
       </c>
-      <c r="P22">
+      <c r="P22" s="4">
         <v>5.99</v>
       </c>
-      <c r="Q22" s="16">
+      <c r="Q22" s="9">
         <v>1.8078703703703704E-2</v>
       </c>
-      <c r="R22" t="s">
+      <c r="R22" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="S22" t="s">
+      <c r="S22" s="14" t="s">
         <v>65</v>
       </c>
     </row>
+    <row r="23" spans="1:19" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="41"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="15"/>
+    </row>
     <row r="24" spans="1:19" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="1" t="s">
+      <c r="C24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" s="1" t="s">
+      <c r="E24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H24" s="18">
+      <c r="H24" s="11">
         <v>12182</v>
       </c>
-      <c r="I24" s="14">
+      <c r="I24" s="7">
         <v>486906</v>
       </c>
-      <c r="J24" s="14">
+      <c r="J24" s="7">
         <v>5383451479</v>
       </c>
-      <c r="K24" s="14">
+      <c r="K24" s="7">
         <v>145526</v>
       </c>
-      <c r="L24" t="s">
+      <c r="L24" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="M24" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="N24">
+      <c r="M24" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="N24" s="4">
         <v>103</v>
       </c>
-      <c r="O24">
+      <c r="O24" s="4">
         <v>44.600999999999999</v>
       </c>
-      <c r="P24">
+      <c r="P24" s="4">
         <v>6.18</v>
       </c>
-      <c r="Q24" s="16">
+      <c r="Q24" s="9">
         <v>3.7743055555555557E-2</v>
       </c>
-      <c r="R24" t="s">
+      <c r="R24" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="S24" t="s">
+      <c r="S24" s="14" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:19" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A25" s="21"/>
-      <c r="B25" t="s">
+      <c r="A25" s="40"/>
+      <c r="B25" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C25" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="C25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E25" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="E25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H25" s="18">
+      <c r="H25" s="11">
         <v>12182</v>
       </c>
-      <c r="I25" s="14">
+      <c r="I25" s="7">
         <v>486906</v>
       </c>
-      <c r="J25" s="14">
+      <c r="J25" s="7">
         <v>5385422479</v>
       </c>
-      <c r="K25" s="14">
+      <c r="K25" s="7">
         <v>145580</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L25" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="M25" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="N25" s="14">
+      <c r="M25" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="N25" s="7">
         <v>99</v>
       </c>
-      <c r="O25">
+      <c r="O25" s="4">
         <v>53.1</v>
       </c>
-      <c r="P25">
+      <c r="P25" s="4">
         <v>6.4</v>
       </c>
-      <c r="Q25" s="16">
+      <c r="Q25" s="9">
         <v>3.7430555555555557E-2</v>
       </c>
-      <c r="R25" t="s">
+      <c r="R25" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="S25" t="s">
+      <c r="S25" s="14" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A26" s="21"/>
-      <c r="B26" t="s">
+      <c r="A26" s="40"/>
+      <c r="B26" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C26" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="C26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="E26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="G26" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H26" s="18">
+      <c r="H26" s="11">
         <v>12182</v>
       </c>
-      <c r="I26" s="14">
+      <c r="I26" s="7">
         <v>486906</v>
       </c>
-      <c r="J26" s="14">
+      <c r="J26" s="7">
         <v>5381617781</v>
       </c>
-      <c r="K26" s="14">
+      <c r="K26" s="7">
         <v>145477</v>
       </c>
-      <c r="L26" t="s">
+      <c r="L26" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="M26" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="N26">
+      <c r="M26" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="N26" s="4">
         <v>117</v>
       </c>
-      <c r="O26">
+      <c r="O26" s="4">
         <v>57.128999999999998</v>
       </c>
-      <c r="P26">
+      <c r="P26" s="4">
         <v>5.99</v>
       </c>
-      <c r="Q26" s="16">
+      <c r="Q26" s="9">
         <v>3.9039351851851853E-2</v>
       </c>
-      <c r="R26" t="s">
+      <c r="R26" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="S26" t="s">
+      <c r="S26" s="14" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A27" s="20"/>
-      <c r="B27" s="4" t="s">
+      <c r="A27" s="40"/>
+      <c r="B27" s="35" t="s">
         <v>13</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -2272,108 +2567,129 @@
       <c r="F27" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="G27" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H27" s="18">
+      <c r="H27" s="11">
         <v>12182</v>
       </c>
-      <c r="I27" s="14">
+      <c r="I27" s="7">
         <v>486906</v>
       </c>
-      <c r="J27" s="14">
+      <c r="J27" s="7">
         <v>5416476615</v>
       </c>
-      <c r="K27" s="14">
+      <c r="K27" s="7">
         <v>146419</v>
       </c>
-      <c r="L27" t="s">
+      <c r="L27" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="M27" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="N27">
+      <c r="M27" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="N27" s="4">
         <v>106</v>
       </c>
-      <c r="O27">
+      <c r="O27" s="4">
         <v>45.325000000000003</v>
       </c>
-      <c r="P27">
+      <c r="P27" s="4">
         <v>7.5</v>
       </c>
-      <c r="Q27" s="16">
+      <c r="Q27" s="9">
         <v>3.876157407407408E-2</v>
       </c>
-      <c r="R27" t="s">
+      <c r="R27" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="S27" t="s">
+      <c r="S27" s="14" t="s">
         <v>107</v>
       </c>
     </row>
+    <row r="28" spans="1:19" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="41"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="12"/>
+      <c r="S28" s="15"/>
+    </row>
     <row r="29" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29" s="1" t="s">
+      <c r="C29" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H29" s="18">
+      <c r="F29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H29" s="11">
         <v>12182</v>
       </c>
-      <c r="I29" s="14">
+      <c r="I29" s="7">
         <v>486906</v>
       </c>
-      <c r="J29" s="14">
+      <c r="J29" s="7">
         <v>58828879</v>
       </c>
-      <c r="K29" s="14">
+      <c r="K29" s="7">
         <v>4828</v>
       </c>
-      <c r="L29" t="s">
+      <c r="L29" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="M29" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="N29">
+      <c r="M29" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="N29" s="4">
         <v>91</v>
       </c>
-      <c r="O29">
+      <c r="O29" s="4">
         <v>13.36</v>
       </c>
-      <c r="P29">
+      <c r="P29" s="4">
         <v>5.99</v>
       </c>
-      <c r="Q29" s="16">
+      <c r="Q29" s="9">
         <v>1.7523148148148149E-2</v>
       </c>
-      <c r="R29" t="s">
+      <c r="R29" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="S29" t="s">
+      <c r="S29" s="14" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A30" s="20"/>
-      <c r="B30" s="4" t="s">
+      <c r="A30" s="40"/>
+      <c r="B30" s="35" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -2388,273 +2704,294 @@
       <c r="F30" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G30" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H30" s="18">
+      <c r="G30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" s="11">
         <v>12182</v>
       </c>
-      <c r="I30" s="14">
+      <c r="I30" s="7">
         <v>486906</v>
       </c>
-      <c r="J30" s="14">
+      <c r="J30" s="7">
         <v>58828879</v>
       </c>
-      <c r="K30" s="14">
+      <c r="K30" s="7">
         <v>4828</v>
       </c>
-      <c r="L30" t="s">
+      <c r="L30" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="M30" s="12" t="s">
+      <c r="M30" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="N30" s="4">
+        <v>122</v>
+      </c>
+      <c r="O30" s="4">
+        <v>19.73</v>
+      </c>
+      <c r="P30" s="4">
+        <v>5.99</v>
+      </c>
+      <c r="Q30" s="9">
+        <v>1.6689814814814817E-2</v>
+      </c>
+      <c r="R30" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="S30" s="14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="41"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="12"/>
+      <c r="R31" s="12"/>
+      <c r="S31" s="15"/>
+    </row>
+    <row r="32" spans="1:19" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A32" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H32" s="11">
+        <v>12182</v>
+      </c>
+      <c r="I32" s="7">
+        <v>486906</v>
+      </c>
+      <c r="J32" s="7">
+        <v>73453103</v>
+      </c>
+      <c r="K32" s="7">
+        <v>6028</v>
+      </c>
+      <c r="L32" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="M32" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="N32" s="4">
+        <v>119</v>
+      </c>
+      <c r="O32" s="4">
+        <v>3.35</v>
+      </c>
+      <c r="P32" s="4">
+        <v>4.97</v>
+      </c>
+      <c r="Q32" s="9">
+        <v>1.8935185185185183E-2</v>
+      </c>
+      <c r="R32" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="S32" s="14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A33" s="40"/>
+      <c r="B33" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H33" s="11">
+        <v>12182</v>
+      </c>
+      <c r="I33" s="7">
+        <v>486906</v>
+      </c>
+      <c r="J33" s="7">
+        <v>73452937</v>
+      </c>
+      <c r="K33" s="7">
+        <v>6028</v>
+      </c>
+      <c r="L33" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="M33" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="N30">
-        <v>122</v>
-      </c>
-      <c r="O30">
-        <v>19.73</v>
-      </c>
-      <c r="P30">
-        <v>5.99</v>
-      </c>
-      <c r="Q30" s="16">
-        <v>1.6689814814814817E-2</v>
-      </c>
-      <c r="R30" t="s">
-        <v>99</v>
-      </c>
-      <c r="S30" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A32" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" s="1" t="s">
+      <c r="N33" s="7">
+        <v>111</v>
+      </c>
+      <c r="O33" s="4">
+        <v>9.3360000000000003</v>
+      </c>
+      <c r="P33" s="4">
+        <v>4.97</v>
+      </c>
+      <c r="Q33" s="9">
+        <v>1.8472222222222223E-2</v>
+      </c>
+      <c r="R33" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="S33" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A34" s="40"/>
+      <c r="B34" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E34" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H32" s="18">
+      <c r="F34" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" s="11">
         <v>12182</v>
       </c>
-      <c r="I32" s="14">
+      <c r="I34" s="7">
         <v>486906</v>
       </c>
-      <c r="J32" s="14">
-        <v>73453103</v>
-      </c>
-      <c r="K32" s="14">
+      <c r="J34" s="7">
+        <v>73454861</v>
+      </c>
+      <c r="K34" s="7">
         <v>6028</v>
       </c>
-      <c r="L32" t="s">
-        <v>90</v>
-      </c>
-      <c r="M32" s="12" t="s">
+      <c r="L34" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="M34" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="N32">
-        <v>119</v>
-      </c>
-      <c r="O32">
-        <v>3.35</v>
-      </c>
-      <c r="P32">
+      <c r="N34" s="4">
+        <v>106</v>
+      </c>
+      <c r="O34" s="4">
+        <v>6.1470000000000002</v>
+      </c>
+      <c r="P34" s="4">
         <v>4.97</v>
       </c>
-      <c r="Q32" s="16">
-        <v>1.8935185185185183E-2</v>
-      </c>
-      <c r="R32" t="s">
-        <v>100</v>
-      </c>
-      <c r="S32" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A33" s="21"/>
-      <c r="B33" t="s">
-        <v>12</v>
-      </c>
-      <c r="C33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="Q34" s="9">
+        <v>1.834490740740741E-2</v>
+      </c>
+      <c r="R34" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="S34" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" ht="85.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A35" s="42"/>
+      <c r="B35" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E35" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F33" t="s">
-        <v>20</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H33" s="18">
+      <c r="F35" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H35" s="17">
         <v>12182</v>
       </c>
-      <c r="I33" s="14">
+      <c r="I35" s="18">
         <v>486906</v>
       </c>
-      <c r="J33" s="14">
-        <v>73452937</v>
-      </c>
-      <c r="K33" s="14">
+      <c r="J35" s="18">
+        <v>73458508</v>
+      </c>
+      <c r="K35" s="18">
         <v>6028</v>
       </c>
-      <c r="L33" t="s">
-        <v>91</v>
-      </c>
-      <c r="M33" s="12" t="s">
+      <c r="L35" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="M35" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="N33" s="14">
-        <v>111</v>
-      </c>
-      <c r="O33">
-        <v>9.3360000000000003</v>
-      </c>
-      <c r="P33">
+      <c r="N35" s="18">
+        <v>114</v>
+      </c>
+      <c r="O35" s="18">
+        <v>5.6219999999999999</v>
+      </c>
+      <c r="P35" s="16">
         <v>4.97</v>
       </c>
-      <c r="Q33" s="16">
-        <v>1.8472222222222223E-2</v>
-      </c>
-      <c r="R33" t="s">
-        <v>102</v>
-      </c>
-      <c r="S33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A34" s="21"/>
-      <c r="B34" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" t="s">
-        <v>15</v>
-      </c>
-      <c r="D34" t="s">
-        <v>23</v>
-      </c>
-      <c r="E34" t="s">
-        <v>17</v>
-      </c>
-      <c r="F34" t="s">
-        <v>20</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H34" s="18">
-        <v>12182</v>
-      </c>
-      <c r="I34" s="14">
-        <v>486906</v>
-      </c>
-      <c r="J34" s="14">
-        <v>73454861</v>
-      </c>
-      <c r="K34" s="14">
-        <v>6028</v>
-      </c>
-      <c r="L34" t="s">
-        <v>92</v>
-      </c>
-      <c r="M34" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="N34">
-        <v>106</v>
-      </c>
-      <c r="O34">
-        <v>6.1470000000000002</v>
-      </c>
-      <c r="P34">
-        <v>4.97</v>
-      </c>
-      <c r="Q34" s="16">
-        <v>1.834490740740741E-2</v>
-      </c>
-      <c r="R34" t="s">
-        <v>101</v>
-      </c>
-      <c r="S34" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A35" s="20"/>
-      <c r="B35" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H35" s="18">
-        <v>12182</v>
-      </c>
-      <c r="I35" s="14">
-        <v>486906</v>
-      </c>
-      <c r="J35" s="14">
-        <v>73458508</v>
-      </c>
-      <c r="K35" s="14">
-        <v>6028</v>
-      </c>
-      <c r="L35" t="s">
-        <v>93</v>
-      </c>
-      <c r="M35" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="N35" s="14">
-        <v>114</v>
-      </c>
-      <c r="O35" s="14">
-        <v>5.6219999999999999</v>
-      </c>
-      <c r="P35">
-        <v>4.97</v>
-      </c>
-      <c r="Q35" s="16">
+      <c r="Q35" s="20">
         <v>1.7465277777777777E-2</v>
       </c>
-      <c r="R35" t="s">
+      <c r="R35" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="S35" t="s">
+      <c r="S35" s="21" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2679,7 +3016,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="A32:A35"/>
     <mergeCell ref="A4:A6"/>

</xml_diff>